<commit_message>
Uploaded database design excel sheet
</commit_message>
<xml_diff>
--- a/Database/Helperland_Database_Sheet.xlsx
+++ b/Database/Helperland_Database_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\tatvasoft\work\Tatvasoft-PSD-TO-HTML\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4158C0D8-85EA-4FAD-B549-A2B8F89CB58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863188A6-657F-49F0-9408-ACF74B3AD1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="821" activeTab="11" xr2:uid="{05D708AD-47AF-4316-B442-EC7D95D66858}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="821" activeTab="4" xr2:uid="{05D708AD-47AF-4316-B442-EC7D95D66858}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
   <si>
     <t>Users</t>
   </si>
@@ -306,12 +306,6 @@
   </si>
   <si>
     <t>favorite_user</t>
-  </si>
-  <si>
-    <t>extra_service_id</t>
-  </si>
-  <si>
-    <t>Foregin Key (ExtraService-&gt;extra_id)</t>
   </si>
   <si>
     <t>extra_id</t>
@@ -893,7 +887,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>28</v>
@@ -1080,7 +1074,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
@@ -1126,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B360051-1F9D-4F68-962F-3DB53B9E99FB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1179,7 +1173,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>
@@ -1188,7 +1182,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>28</v>
@@ -1473,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E79D86-BED5-4DAC-A1B6-CAD800B351C5}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1555,56 +1549,54 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
@@ -1613,36 +1605,27 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1669,7 +1652,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1687,7 +1670,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1709,7 +1692,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>
@@ -1718,7 +1701,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1727,7 +1710,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added UserType table from Users
</commit_message>
<xml_diff>
--- a/Database/Helperland_Database_Sheet.xlsx
+++ b/Database/Helperland_Database_Sheet.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\tatvasoft\work\Tatvasoft-PSD-TO-HTML\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863188A6-657F-49F0-9408-ACF74B3AD1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA55B4-8E3A-4F12-B5BA-5C58B7CD9486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="821" activeTab="4" xr2:uid="{05D708AD-47AF-4316-B442-EC7D95D66858}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="821" activeTab="9" xr2:uid="{05D708AD-47AF-4316-B442-EC7D95D66858}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
-    <sheet name="UserServicer" sheetId="3" r:id="rId2"/>
-    <sheet name="UserAddress" sheetId="4" r:id="rId3"/>
-    <sheet name="City" sheetId="5" r:id="rId4"/>
-    <sheet name="Service" sheetId="8" r:id="rId5"/>
-    <sheet name="ExtraService" sheetId="15" r:id="rId6"/>
-    <sheet name="ServiceHistory" sheetId="9" r:id="rId7"/>
-    <sheet name="UsersFavorites" sheetId="12" r:id="rId8"/>
-    <sheet name="ServiceRating" sheetId="10" r:id="rId9"/>
-    <sheet name="FAQs" sheetId="6" r:id="rId10"/>
-    <sheet name="ContactMessage" sheetId="7" r:id="rId11"/>
-    <sheet name="Notification" sheetId="14" r:id="rId12"/>
+    <sheet name="UserType" sheetId="16" r:id="rId2"/>
+    <sheet name="UserServicer" sheetId="3" r:id="rId3"/>
+    <sheet name="UserAddress" sheetId="4" r:id="rId4"/>
+    <sheet name="City" sheetId="5" r:id="rId5"/>
+    <sheet name="Service" sheetId="8" r:id="rId6"/>
+    <sheet name="ExtraService" sheetId="15" r:id="rId7"/>
+    <sheet name="ServiceHistory" sheetId="9" r:id="rId8"/>
+    <sheet name="UsersFavorites" sheetId="12" r:id="rId9"/>
+    <sheet name="ServiceRating" sheetId="10" r:id="rId10"/>
+    <sheet name="FAQs" sheetId="6" r:id="rId11"/>
+    <sheet name="ContactMessage" sheetId="7" r:id="rId12"/>
+    <sheet name="Notification" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="100">
   <si>
     <t>Users</t>
   </si>
@@ -89,9 +90,6 @@
     <t>date_of_registration</t>
   </si>
   <si>
-    <t>UserServicer</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
@@ -206,9 +204,6 @@
     <t>address_id</t>
   </si>
   <si>
-    <t>payment</t>
-  </si>
-  <si>
     <t>Service</t>
   </si>
   <si>
@@ -230,9 +225,6 @@
     <t>service_accept_by_id</t>
   </si>
   <si>
-    <t>servicer_id</t>
-  </si>
-  <si>
     <t>Foreign key (Servicer-&gt;servicer_id)</t>
   </si>
   <si>
@@ -333,6 +325,27 @@
   </si>
   <si>
     <t>message_type</t>
+  </si>
+  <si>
+    <t>user_type_id</t>
+  </si>
+  <si>
+    <t>Foreign Key (UserType-&gt;user_type_id)</t>
+  </si>
+  <si>
+    <t>UserType</t>
+  </si>
+  <si>
+    <t>ServiceProvider</t>
+  </si>
+  <si>
+    <t>sp_id</t>
+  </si>
+  <si>
+    <t>payment_status</t>
+  </si>
+  <si>
+    <t>preferred_language</t>
   </si>
 </sst>
 </file>
@@ -762,17 +775,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E073C6D7-D3EB-43BA-80B7-C0022ED1D74B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" customWidth="1"/>
     <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -790,12 +803,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -809,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -818,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -827,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -836,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -845,25 +858,27 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -872,7 +887,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -881,29 +896,38 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
@@ -914,6 +938,114 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF837C9-6137-43DE-851B-331B0470AEFA}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970C01DE-89ED-42A6-84BB-4B114211C0E6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -930,7 +1062,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -943,12 +1075,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -959,28 +1091,28 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -992,7 +1124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EB5958-BB86-41C9-9B66-93117B187D05}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1009,7 +1141,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1022,12 +1154,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1041,16 +1173,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1059,7 +1191,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1068,43 +1200,43 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -1116,7 +1248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B360051-1F9D-4F68-962F-3DB53B9E99FB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1133,7 +1265,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1146,12 +1278,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1162,30 +1294,30 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1198,11 +1330,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F839B64-8825-41BF-AAE7-F5A768B8CE14}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D281B7E8-71B6-433E-B62D-FF06D472FDE1}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1410,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1227,32 +1423,32 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
@@ -1261,10 +1457,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -1285,7 +1481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDF80D0-BEBD-44A5-91BB-134599EDDDAE}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1302,7 +1498,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1315,12 +1511,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1331,59 +1527,59 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1395,7 +1591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9F7E69-4CCD-4594-8823-6A011380A844}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1412,7 +1608,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1425,12 +1621,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1441,7 +1637,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -1450,10 +1646,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1465,12 +1661,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E79D86-BED5-4DAC-A1B6-CAD800B351C5}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,7 +1678,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1495,12 +1691,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1511,45 +1707,45 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -1558,65 +1754,65 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -1635,7 +1831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900C1C7B-55E2-4975-851D-4EECCF970105}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1652,7 +1848,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1665,12 +1861,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1681,27 +1877,27 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1710,7 +1906,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1725,7 +1921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC46D72C-6B17-4F57-8695-69C740E5B0FF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1742,7 +1938,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1755,12 +1951,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -1771,21 +1967,21 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -1797,12 +1993,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B23456-144A-45DB-B18C-99B4A78A1650}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,7 +2010,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1827,170 +2023,62 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF837C9-6137-43DE-851B-331B0470AEFA}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>